<commit_message>
excel file for analysis data set up
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F90A77-40B3-4F6F-A9A3-3D546D41C9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C81566F-285A-42B0-97C3-274318553DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1970" yWindow="750" windowWidth="14400" windowHeight="9350" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Data CSV filename</t>
+  </si>
+  <si>
+    <t>Start array index</t>
+  </si>
+  <si>
+    <t>End array index</t>
+  </si>
+  <si>
+    <t>Start wavelength</t>
+  </si>
+  <si>
+    <t>End wavelength</t>
+  </si>
+  <si>
+    <t>fsr_mean</t>
+  </si>
+  <si>
+    <t>fsr_std error</t>
+  </si>
+  <si>
+    <t>prominence</t>
+  </si>
+  <si>
+    <t>Wavelength step size</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definitions: Data CSV filename: the filename of the scan data read in when doing the analysis.  </t>
+  </si>
+  <si>
+    <t>approx_fsr</t>
+  </si>
+  <si>
+    <t>The analysis aims to take wavelength and power transmission scan data for different structures, to find resonance peaks in this data and then calculate the free spectral range of the structure from this.</t>
+  </si>
+  <si>
+    <t>This is done by finding peaks using scipy.signal.find_peaks(), and then finding the difference in wavelength between these peak locations. This gives a series of wavelength fsrs.</t>
+  </si>
+  <si>
+    <t>Then, this series of wavelength fsrs is used to find its mean. Then the standard error is found by using np.std with ddof=1 to get the standard deviation, and then dividing by square root of number of fsrs in the series.</t>
+  </si>
+  <si>
+    <t>We only use a section of the full data in the CSV files for the peak finding. This is detailed by start array index and end array index (and also start wavelength and end wavelength).</t>
+  </si>
+  <si>
+    <t>Start array index: The index that the arrays of powers and wavelengths used to find resonance peaks starts at ( array includes this item). Note index is for numpy arrayso starts at 0</t>
+  </si>
+  <si>
+    <t>End array index: The index that arrays of powers and wavelengths used to find resonance peaks ends one before (array does not include this index item).</t>
+  </si>
+  <si>
+    <t>Start wavelength: The wavelength that the data used to find peaks starts at. This data point is included in data to find resonance peaks.</t>
+  </si>
+  <si>
+    <t>fsr_mean: the mean free spectral range as calculated by the code from finding resonance peaks as detailed above.</t>
+  </si>
+  <si>
+    <t>fsr_std_error: the standard error in the free spectral range, as calculated by the code from finding resonance peaks as detailed above.</t>
+  </si>
+  <si>
+    <t>The files under team-chip-project are in a Git repo. At the moment working on branch: Tamanna19Dec_analysis.</t>
+  </si>
+  <si>
+    <t>distance:the value passed into scipy.signal.find_peaks when peak finding as the distance parameter. The minimum distance between peaks in number of points. Choose this by taking approx_fsr/2 and dividing that by wavelength step size.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approx_fsr: chosen by looking at plot, and maybe using a ruler, and guessing by eye roughly what the free spectral range is. It is divided by the wavelength step size to give the wlen parameter to be passed into scipy.signal.find_peaks() for finding the peaks. </t>
+  </si>
+  <si>
+    <t>The procedure will be to Git commit after each run and after I've added the parameters to this table, so each commit should contain the state of the code and state of the table after each run has been recorded.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This file records the analysis results that I get when analysing data as shown in the Jupyter Notebook at: "C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis" </t>
+  </si>
+  <si>
+    <t>Wavelength step size: the step size passed into the give_peak_locs function used to calculate the approx_fsr in number of data points rather than wavelength to be passed into scipy.signal.find_peaks() to be used as wlen.</t>
+  </si>
+  <si>
+    <t>End wavelength: The wavelength that the data used to find peaks ends at. This data point is included in the data to find resonance peaks.</t>
+  </si>
+  <si>
+    <t>prominence: the value passed into scipy.signal.find_peaks() when peak finding as the prominence parameter. See notes for exact definition of this. Chosen by looking by eye and picking about half of the height span of a noise part of the graph that doesn't contain the resonance peaks.</t>
   </si>
 </sst>
 </file>
@@ -390,20 +474,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A4"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.08984375" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" t="s">
+        <v>5</v>
+      </c>
+      <c r="K21" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first proper attempt at data analysis, appears to have gone wrong
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C81566F-285A-42B0-97C3-274318553DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A3EB38-C318-4D19-9401-CA93688419C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -47,33 +47,12 @@
     <t>End array index</t>
   </si>
   <si>
-    <t>Start wavelength</t>
-  </si>
-  <si>
-    <t>End wavelength</t>
-  </si>
-  <si>
-    <t>fsr_mean</t>
-  </si>
-  <si>
-    <t>fsr_std error</t>
-  </si>
-  <si>
-    <t>prominence</t>
-  </si>
-  <si>
-    <t>Wavelength step size</t>
-  </si>
-  <si>
     <t>distance</t>
   </si>
   <si>
     <t xml:space="preserve">Definitions: Data CSV filename: the filename of the scan data read in when doing the analysis.  </t>
   </si>
   <si>
-    <t>approx_fsr</t>
-  </si>
-  <si>
     <t>The analysis aims to take wavelength and power transmission scan data for different structures, to find resonance peaks in this data and then calculate the free spectral range of the structure from this.</t>
   </si>
   <si>
@@ -123,6 +102,36 @@
   </si>
   <si>
     <t>prominence: the value passed into scipy.signal.find_peaks() when peak finding as the prominence parameter. See notes for exact definition of this. Chosen by looking by eye and picking about half of the height span of a noise part of the graph that doesn't contain the resonance peaks.</t>
+  </si>
+  <si>
+    <t>sg_rr_20_025 2023-12-13 17-59-26.csv</t>
+  </si>
+  <si>
+    <t>Wavelength step size/nm</t>
+  </si>
+  <si>
+    <t>Start wavelength/nm</t>
+  </si>
+  <si>
+    <t>End wavelength/nm</t>
+  </si>
+  <si>
+    <t>approx_fsr/nm</t>
+  </si>
+  <si>
+    <t>fsr_mean/nm</t>
+  </si>
+  <si>
+    <t>fsr_std error/nm</t>
+  </si>
+  <si>
+    <t>prominence/dBm</t>
+  </si>
+  <si>
+    <t>(approx_fsr/2)/wavelength step size</t>
+  </si>
+  <si>
+    <t>Note, may have to rethink, as it looks like there is an issue with this first analysis when plotted, it seems to have found a peak at the start where visually doesn't seem to be any.</t>
   </si>
 </sst>
 </file>
@@ -158,8 +167,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,121 +484,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.6328125" customWidth="1"/>
+    <col min="2" max="2" width="22.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.08984375" customWidth="1"/>
+    <col min="7" max="7" width="14.08984375" customWidth="1"/>
+    <col min="8" max="8" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.08984375" customWidth="1"/>
+    <col min="10" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -597,28 +610,70 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" t="s">
         <v>3</v>
       </c>
-      <c r="F21" t="s">
-        <v>4</v>
-      </c>
-      <c r="G21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" t="s">
-        <v>9</v>
-      </c>
       <c r="I21" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="J21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>0.01</v>
+      </c>
+      <c r="C22">
+        <v>1000</v>
+      </c>
+      <c r="D22">
+        <v>5001</v>
+      </c>
+      <c r="E22">
+        <v>1530</v>
+      </c>
+      <c r="F22">
+        <v>1570</v>
+      </c>
+      <c r="G22">
+        <v>0.25</v>
+      </c>
+      <c r="H22" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22">
         <v>5</v>
       </c>
-      <c r="K21" t="s">
-        <v>6</v>
-      </c>
+      <c r="J22">
+        <v>4.7075000000000102</v>
+      </c>
+      <c r="K22">
+        <v>0.213631441639898</v>
+      </c>
+      <c r="L22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data run of first data set with higher prominence
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A3EB38-C318-4D19-9401-CA93688419C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED9D703-618D-467B-83CD-9E8E0FE9980A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>Note, may have to rethink, as it looks like there is an issue with this first analysis when plotted, it seems to have found a peak at the start where visually doesn't seem to be any.</t>
+  </si>
+  <si>
+    <t>Actually note, this way of choosing the prominence seemed not to work for first data run, so from now, will put a note about how prominence was selected for each run next to its row in the table. Probably going to try and aim for maybe the whole height span of visually looking roughly the widest noise part that doesn't seem to visually contain a peak.</t>
+  </si>
+  <si>
+    <t>Also note, if things change between the runs, will try to note this next to data row.</t>
+  </si>
+  <si>
+    <t>Note I think Excel is not storing full number digits as printed out in Jupyter notebook, as I copy and paste the fsr mean and error into here, but it is keeping enough significant figures, and we should be able to look to GitHub or run data again.</t>
   </si>
 </sst>
 </file>
@@ -169,7 +178,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,94 +594,139 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" t="s">
         <v>2</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>24</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F23" t="s">
         <v>25</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G23" t="s">
         <v>29</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H23" t="s">
         <v>3</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I23" t="s">
         <v>26</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J23" t="s">
         <v>27</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>0.01</v>
       </c>
-      <c r="C22">
+      <c r="C24">
         <v>1000</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>5001</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>1530</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <v>1570</v>
       </c>
-      <c r="G22">
+      <c r="G24">
         <v>0.25</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H24" t="s">
         <v>30</v>
       </c>
-      <c r="I22">
+      <c r="I24">
         <v>5</v>
       </c>
-      <c r="J22">
+      <c r="J24">
         <v>4.7075000000000102</v>
       </c>
-      <c r="K22">
+      <c r="K24">
         <v>0.213631441639898</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="J23" s="1"/>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>0.01</v>
+      </c>
+      <c r="C25">
+        <v>1000</v>
+      </c>
+      <c r="D25">
+        <v>5001</v>
+      </c>
+      <c r="E25">
+        <v>1530</v>
+      </c>
+      <c r="F25">
+        <v>1570</v>
+      </c>
+      <c r="G25">
+        <v>0.5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
+      <c r="J25" s="1">
+        <v>4.92</v>
+      </c>
+      <c r="K25">
+        <v>2.5354627641843101E-2</v>
+      </c>
+      <c r="L25" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
next data run looks to have picked up noise as well
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED9D703-618D-467B-83CD-9E8E0FE9980A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF7C7DA-0C38-4731-9D44-9C8314A3204C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>Note I think Excel is not storing full number digits as printed out in Jupyter notebook, as I copy and paste the fsr mean and error into here, but it is keeping enough significant figures, and we should be able to look to GitHub or run data again.</t>
+  </si>
+  <si>
+    <t>sg_rr_36_025 2023-12-13 16-41-08</t>
+  </si>
+  <si>
+    <t>prominence set by looking at roughly biggest height span of noise bits that don't appear visually to contain resonance peaks</t>
   </si>
 </sst>
 </file>
@@ -495,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,6 +734,44 @@
         <v>34</v>
       </c>
     </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>0.01</v>
+      </c>
+      <c r="C26">
+        <v>1000</v>
+      </c>
+      <c r="D26">
+        <v>5001</v>
+      </c>
+      <c r="E26">
+        <v>1530</v>
+      </c>
+      <c r="F26">
+        <v>1570</v>
+      </c>
+      <c r="G26">
+        <v>0.5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26">
+        <v>2.5</v>
+      </c>
+      <c r="J26">
+        <v>2.5459999999999998</v>
+      </c>
+      <c r="K26">
+        <v>0.12551152479809299</v>
+      </c>
+      <c r="L26" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
repeating previous run with higher prominence
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF7C7DA-0C38-4731-9D44-9C8314A3204C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A19A5B0-2244-4043-99D0-E962CF0E7514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -143,10 +143,13 @@
     <t>Note I think Excel is not storing full number digits as printed out in Jupyter notebook, as I copy and paste the fsr mean and error into here, but it is keeping enough significant figures, and we should be able to look to GitHub or run data again.</t>
   </si>
   <si>
-    <t>sg_rr_36_025 2023-12-13 16-41-08</t>
-  </si>
-  <si>
     <t>prominence set by looking at roughly biggest height span of noise bits that don't appear visually to contain resonance peaks</t>
+  </si>
+  <si>
+    <t>sg_rr_36_025 2023-12-13 16-41-08.csv</t>
+  </si>
+  <si>
+    <t>just increasing prominence slightly from previous run as visually it seemed to find noise.</t>
   </si>
 </sst>
 </file>
@@ -501,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -736,7 +739,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>0.01</v>
@@ -769,7 +772,45 @@
         <v>0.12551152479809299</v>
       </c>
       <c r="L26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>36</v>
+      </c>
+      <c r="B27">
+        <v>0.01</v>
+      </c>
+      <c r="C27">
+        <v>1000</v>
+      </c>
+      <c r="D27">
+        <v>5001</v>
+      </c>
+      <c r="E27">
+        <v>1530</v>
+      </c>
+      <c r="F27">
+        <v>1570</v>
+      </c>
+      <c r="G27">
+        <v>0.6</v>
+      </c>
+      <c r="H27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27">
+        <v>2.5</v>
+      </c>
+      <c r="J27">
+        <v>2.7278571428571401</v>
+      </c>
+      <c r="K27">
+        <v>1.3390933927838499E-2</v>
+      </c>
+      <c r="L27" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a data run on sg_rr_100_027
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BDFE8C-E88B-4101-B916-792684609843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D956184E-B3E3-4C3F-B50A-EDAEC14DF5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -189,6 +189,15 @@
   </si>
   <si>
     <t>yes (no double counting, but last peak maybe missed, although unclear if that's a peak)</t>
+  </si>
+  <si>
+    <t>sg_rr_100_027 2023-12-08 17-44-55.csv</t>
+  </si>
+  <si>
+    <t>prominence kept same, thought about increasing a little when trying to look roughly by eye for roughly biggest height span of noisy bit containing no peaks but decide to keep it same and adjust slightly if need be, as looks roughly right anyway, and wouldn't want to increase it unnecessarily if not needed.</t>
+  </si>
+  <si>
+    <t>yes (no double-counting but possible loss of last peak as it is on edge)</t>
   </si>
 </sst>
 </file>
@@ -543,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1022,6 +1031,47 @@
         <v>49</v>
       </c>
     </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33">
+        <v>0.01</v>
+      </c>
+      <c r="C33">
+        <v>1000</v>
+      </c>
+      <c r="D33">
+        <v>5001</v>
+      </c>
+      <c r="E33">
+        <v>1530</v>
+      </c>
+      <c r="F33">
+        <v>1570</v>
+      </c>
+      <c r="G33">
+        <v>0.5</v>
+      </c>
+      <c r="H33" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33">
+        <v>1.7</v>
+      </c>
+      <c r="J33">
+        <v>0.98153846153846003</v>
+      </c>
+      <c r="K33">
+        <v>4.3858818636388196E-3</v>
+      </c>
+      <c r="L33" t="s">
+        <v>53</v>
+      </c>
+      <c r="M33" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
data run for sg_rr_100_028
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D956184E-B3E3-4C3F-B50A-EDAEC14DF5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3669BD-2F59-48BE-8923-871341462FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="9350" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -198,6 +198,15 @@
   </si>
   <si>
     <t>yes (no double-counting but possible loss of last peak as it is on edge)</t>
+  </si>
+  <si>
+    <t>sg_rr_100_028 2023-12-08 16-58-05.csv</t>
+  </si>
+  <si>
+    <t>prominence left at 0.5, as height span of noisy parts of data looks roughly around this value roughly at its max span looking by eye at a glance.</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -552,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1072,6 +1081,47 @@
         <v>52</v>
       </c>
     </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34">
+        <v>0.01</v>
+      </c>
+      <c r="C34">
+        <v>1000</v>
+      </c>
+      <c r="D34">
+        <v>5001</v>
+      </c>
+      <c r="E34">
+        <v>1530</v>
+      </c>
+      <c r="F34">
+        <v>1570</v>
+      </c>
+      <c r="G34">
+        <v>0.5</v>
+      </c>
+      <c r="H34" t="s">
+        <v>30</v>
+      </c>
+      <c r="I34">
+        <v>1.7</v>
+      </c>
+      <c r="J34">
+        <v>0.98274999999999801</v>
+      </c>
+      <c r="K34">
+        <v>3.2814064370514399E-3</v>
+      </c>
+      <c r="L34" t="s">
+        <v>56</v>
+      </c>
+      <c r="M34" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
data run for sg_rr_100_030 2023-12-08 16-08-32
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3669BD-2F59-48BE-8923-871341462FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D20D387-239E-46D8-A57F-AF019FC72404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="9350" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>sg_rr_100_030 2023-12-08 16-08-32.csv</t>
   </si>
 </sst>
 </file>
@@ -561,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1122,6 +1125,47 @@
         <v>55</v>
       </c>
     </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35">
+        <v>0.01</v>
+      </c>
+      <c r="C35">
+        <v>1000</v>
+      </c>
+      <c r="D35">
+        <v>5001</v>
+      </c>
+      <c r="E35">
+        <v>1530</v>
+      </c>
+      <c r="F35">
+        <v>1570</v>
+      </c>
+      <c r="G35">
+        <v>0.5</v>
+      </c>
+      <c r="H35" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>0.98128205128205004</v>
+      </c>
+      <c r="K35">
+        <v>3.16397329552258E-3</v>
+      </c>
+      <c r="L35" t="s">
+        <v>56</v>
+      </c>
+      <c r="M35" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Went back to old commits and checked for peak double-counting and added to table
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D20D387-239E-46D8-A57F-AF019FC72404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529E2729-6C33-4E23-8662-A086A8001332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>sg_rr_100_030 2023-12-08 16-08-32.csv</t>
+  </si>
+  <si>
+    <t>Going back in Git commits, to check the files I forgot to check for peak double-counting</t>
+  </si>
+  <si>
+    <t>yes looking back at Git history of notebook</t>
   </si>
 </sst>
 </file>
@@ -564,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,7 +589,7 @@
     <col min="9" max="9" width="14.08984375" customWidth="1"/>
     <col min="10" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.26953125" customWidth="1"/>
+    <col min="12" max="12" width="74.08984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -692,123 +698,52 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" t="s">
-        <v>26</v>
-      </c>
-      <c r="J24" t="s">
-        <v>27</v>
-      </c>
-      <c r="K24" t="s">
-        <v>28</v>
-      </c>
-      <c r="L24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25">
-        <v>0.01</v>
-      </c>
-      <c r="C25">
-        <v>1000</v>
-      </c>
-      <c r="D25">
-        <v>5001</v>
-      </c>
-      <c r="E25">
-        <v>1530</v>
-      </c>
-      <c r="F25">
-        <v>1570</v>
-      </c>
-      <c r="G25">
-        <v>0.25</v>
-      </c>
-      <c r="H25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25">
-        <v>5</v>
-      </c>
-      <c r="J25">
-        <v>4.7075000000000102</v>
-      </c>
-      <c r="K25">
-        <v>0.213631441639898</v>
-      </c>
-      <c r="M25" t="s">
-        <v>31</v>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26">
-        <v>0.01</v>
-      </c>
-      <c r="C26">
-        <v>1000</v>
-      </c>
-      <c r="D26">
-        <v>5001</v>
-      </c>
-      <c r="E26">
-        <v>1530</v>
-      </c>
-      <c r="F26">
-        <v>1570</v>
-      </c>
-      <c r="G26">
-        <v>0.5</v>
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" t="s">
+        <v>29</v>
       </c>
       <c r="H26" t="s">
-        <v>30</v>
-      </c>
-      <c r="I26">
-        <v>5</v>
-      </c>
-      <c r="J26" s="1">
-        <v>4.92</v>
-      </c>
-      <c r="K26">
-        <v>2.5354627641843101E-2</v>
-      </c>
-      <c r="M26" t="s">
-        <v>34</v>
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" t="s">
+        <v>28</v>
+      </c>
+      <c r="L26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B27">
         <v>0.01</v>
@@ -826,27 +761,30 @@
         <v>1570</v>
       </c>
       <c r="G27">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="H27" t="s">
         <v>30</v>
       </c>
       <c r="I27">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="J27">
-        <v>2.5459999999999998</v>
+        <v>4.7075000000000102</v>
       </c>
       <c r="K27">
-        <v>0.12551152479809299</v>
+        <v>0.213631441639898</v>
+      </c>
+      <c r="L27" t="s">
+        <v>59</v>
       </c>
       <c r="M27" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B28">
         <v>0.01</v>
@@ -864,27 +802,30 @@
         <v>1570</v>
       </c>
       <c r="G28">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="H28" t="s">
         <v>30</v>
       </c>
       <c r="I28">
-        <v>2.5</v>
-      </c>
-      <c r="J28">
-        <v>2.7278571428571401</v>
+        <v>5</v>
+      </c>
+      <c r="J28" s="1">
+        <v>4.92</v>
       </c>
       <c r="K28">
-        <v>1.3390933927838499E-2</v>
+        <v>2.5354627641843101E-2</v>
+      </c>
+      <c r="L28" t="s">
+        <v>59</v>
       </c>
       <c r="M28" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29">
         <v>0.01</v>
@@ -911,18 +852,21 @@
         <v>2.5</v>
       </c>
       <c r="J29">
-        <v>1.8875</v>
+        <v>2.5459999999999998</v>
       </c>
       <c r="K29">
-        <v>7.8430324425366096E-3</v>
+        <v>0.12551152479809299</v>
+      </c>
+      <c r="L29" t="s">
+        <v>59</v>
       </c>
       <c r="M29" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B30">
         <v>0.01</v>
@@ -940,30 +884,30 @@
         <v>1570</v>
       </c>
       <c r="G30">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="H30" t="s">
         <v>30</v>
       </c>
       <c r="I30">
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="J30">
-        <v>1.4480769230769099</v>
+        <v>2.7278571428571401</v>
       </c>
       <c r="K30">
-        <v>6.22696940163916E-3</v>
+        <v>1.3390933927838499E-2</v>
       </c>
       <c r="L30" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="M30" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B31">
         <v>0.01</v>
@@ -987,24 +931,24 @@
         <v>30</v>
       </c>
       <c r="I31">
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="J31">
-        <v>1.1724242424242399</v>
+        <v>1.8875</v>
       </c>
       <c r="K31">
-        <v>5.9834098769671303E-3</v>
+        <v>7.8430324425366096E-3</v>
       </c>
       <c r="L31" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="M31" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B32">
         <v>0.01</v>
@@ -1031,21 +975,21 @@
         <v>1.7</v>
       </c>
       <c r="J32">
-        <v>0.98282051282051597</v>
+        <v>1.4480769230769099</v>
       </c>
       <c r="K32">
-        <v>5.5097596875867197E-3</v>
+        <v>6.22696940163916E-3</v>
       </c>
       <c r="L32" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="M32" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B33">
         <v>0.01</v>
@@ -1072,21 +1016,21 @@
         <v>1.7</v>
       </c>
       <c r="J33">
-        <v>0.98153846153846003</v>
+        <v>1.1724242424242399</v>
       </c>
       <c r="K33">
-        <v>4.3858818636388196E-3</v>
+        <v>5.9834098769671303E-3</v>
       </c>
       <c r="L33" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="M33" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B34">
         <v>0.01</v>
@@ -1113,21 +1057,21 @@
         <v>1.7</v>
       </c>
       <c r="J34">
-        <v>0.98274999999999801</v>
+        <v>0.98282051282051597</v>
       </c>
       <c r="K34">
-        <v>3.2814064370514399E-3</v>
+        <v>5.5097596875867197E-3</v>
       </c>
       <c r="L34" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="M34" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B35">
         <v>0.01</v>
@@ -1151,18 +1095,100 @@
         <v>30</v>
       </c>
       <c r="I35">
+        <v>1.7</v>
+      </c>
+      <c r="J35">
+        <v>0.98153846153846003</v>
+      </c>
+      <c r="K35">
+        <v>4.3858818636388196E-3</v>
+      </c>
+      <c r="L35" t="s">
+        <v>53</v>
+      </c>
+      <c r="M35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36">
+        <v>0.01</v>
+      </c>
+      <c r="C36">
+        <v>1000</v>
+      </c>
+      <c r="D36">
+        <v>5001</v>
+      </c>
+      <c r="E36">
+        <v>1530</v>
+      </c>
+      <c r="F36">
+        <v>1570</v>
+      </c>
+      <c r="G36">
+        <v>0.5</v>
+      </c>
+      <c r="H36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36">
+        <v>1.7</v>
+      </c>
+      <c r="J36">
+        <v>0.98274999999999801</v>
+      </c>
+      <c r="K36">
+        <v>3.2814064370514399E-3</v>
+      </c>
+      <c r="L36" t="s">
+        <v>56</v>
+      </c>
+      <c r="M36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37">
+        <v>0.01</v>
+      </c>
+      <c r="C37">
+        <v>1000</v>
+      </c>
+      <c r="D37">
+        <v>5001</v>
+      </c>
+      <c r="E37">
+        <v>1530</v>
+      </c>
+      <c r="F37">
+        <v>1570</v>
+      </c>
+      <c r="G37">
+        <v>0.5</v>
+      </c>
+      <c r="H37" t="s">
+        <v>30</v>
+      </c>
+      <c r="I37">
         <v>1</v>
       </c>
-      <c r="J35">
+      <c r="J37">
         <v>0.98128205128205004</v>
       </c>
-      <c r="K35">
+      <c r="K37">
         <v>3.16397329552258E-3</v>
       </c>
-      <c r="L35" t="s">
+      <c r="L37" t="s">
         <v>56</v>
       </c>
-      <c r="M35" t="s">
+      <c r="M37" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
trying fsr data run for sg_rr_20_025 2023-12-13 17-59-26 with distance set to 1 to see what happens
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529E2729-6C33-4E23-8662-A086A8001332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0929F23A-1156-44FB-8BA3-D34D129E25C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -216,19 +216,33 @@
   </si>
   <si>
     <t>yes looking back at Git history of notebook</t>
+  </si>
+  <si>
+    <t>May try also some runs with distance=1, just to see if it still works, and whether it can find peaks without double-counting.</t>
+  </si>
+  <si>
+    <t>yes but looks to have also found peaks in noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prominence setto be same as a previous run </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -251,11 +265,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -703,6 +718,11 @@
         <v>58</v>
       </c>
     </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>0</v>
@@ -1190,6 +1210,47 @@
       </c>
       <c r="M37" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39">
+        <v>0.01</v>
+      </c>
+      <c r="C39">
+        <v>1000</v>
+      </c>
+      <c r="D39">
+        <v>5001</v>
+      </c>
+      <c r="E39">
+        <v>1530</v>
+      </c>
+      <c r="F39">
+        <v>1570</v>
+      </c>
+      <c r="G39">
+        <v>0.5</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>5</v>
+      </c>
+      <c r="J39">
+        <v>3.0433333333333299</v>
+      </c>
+      <c r="K39" s="2">
+        <v>0.58130382883148601</v>
+      </c>
+      <c r="L39" t="s">
+        <v>61</v>
+      </c>
+      <c r="M39" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unsure what modification was made to excel file so just committing anyway
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0929F23A-1156-44FB-8BA3-D34D129E25C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D7A6AA-AEE9-47A1-9875-04D420F4E1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -588,7 +588,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
don't think I changed excel file but committing anyway
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D7A6AA-AEE9-47A1-9875-04D420F4E1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF926A4-78B5-44B8-A4CD-BEDC62D404CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -588,7 +588,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
setting up excel file ready for FWHM runs
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF926A4-78B5-44B8-A4CD-BEDC62D404CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA88CC2-2960-49E3-900A-C606C647401C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -225,6 +225,36 @@
   </si>
   <si>
     <t xml:space="preserve">prominence setto be same as a previous run </t>
+  </si>
+  <si>
+    <t>scipy.signal.peak_widths is used to do this with the parameter rel_height=0.5. This means peak width is found at h=h_peak-PR where h_peak is the height of the peaks (note the peaks are found by flipping the resonance data because the resonances are minima).</t>
+  </si>
+  <si>
+    <t>The analysis results shown below are for looking for the average FWHM for the scan data of the structures. I use the same Jupyter Notebook as above.</t>
+  </si>
+  <si>
+    <t>scipy.signal.peak_widths is found in samples, and multiplied by wavelength_step_size to give the FWHM in nm</t>
+  </si>
+  <si>
+    <t>Data CSV Filename</t>
+  </si>
+  <si>
+    <t>peak data is found in same way as above</t>
+  </si>
+  <si>
+    <t>FWHM error/nm</t>
+  </si>
+  <si>
+    <t>mean FWHM/nm</t>
+  </si>
+  <si>
+    <t>definitions unless stated otherwise are same as above. I will also add the fsr data below as I might as well, because notebook calculates both fsr and FWHM data.</t>
+  </si>
+  <si>
+    <t>I will Git commit after each data run and entry into this table.</t>
+  </si>
+  <si>
+    <t>The parameter wlen passed into peak_widths is approx_fsr/wavelength step size</t>
   </si>
 </sst>
 </file>
@@ -585,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,15 +627,16 @@
     <col min="2" max="2" width="22.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.08984375" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.08984375" customWidth="1"/>
     <col min="10" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="74.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.36328125" customWidth="1"/>
+    <col min="14" max="14" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -1253,6 +1284,85 @@
         <v>62</v>
       </c>
     </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" t="s">
+        <v>29</v>
+      </c>
+      <c r="H53" t="s">
+        <v>3</v>
+      </c>
+      <c r="I53" t="s">
+        <v>26</v>
+      </c>
+      <c r="J53" t="s">
+        <v>27</v>
+      </c>
+      <c r="K53" t="s">
+        <v>28</v>
+      </c>
+      <c r="L53" t="s">
+        <v>43</v>
+      </c>
+      <c r="M53" t="s">
+        <v>69</v>
+      </c>
+      <c r="N53" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FWHM data run for sg_rr_20_025 2023-12-13 17-59-26
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA88CC2-2960-49E3-900A-C606C647401C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B77C99-A6C8-4E95-87A8-517116D571FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -239,9 +239,6 @@
     <t>Data CSV Filename</t>
   </si>
   <si>
-    <t>peak data is found in same way as above</t>
-  </si>
-  <si>
     <t>FWHM error/nm</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>The parameter wlen passed into peak_widths is approx_fsr/wavelength step size</t>
+  </si>
+  <si>
+    <t>peak data is found in same way as above although may adjust parameters like approx_fsr if see fit</t>
   </si>
 </sst>
 </file>
@@ -615,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="76" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,7 +634,7 @@
     <col min="9" max="9" width="14.08984375" customWidth="1"/>
     <col min="10" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="74.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
     <col min="13" max="13" width="15.36328125" customWidth="1"/>
     <col min="14" max="14" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1301,22 +1301,22 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
@@ -1357,10 +1357,54 @@
         <v>43</v>
       </c>
       <c r="M53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N53" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54">
+        <v>0.01</v>
+      </c>
+      <c r="C54">
+        <v>1000</v>
+      </c>
+      <c r="D54">
+        <v>5001</v>
+      </c>
+      <c r="E54">
+        <v>1530</v>
+      </c>
+      <c r="F54">
+        <v>1570</v>
+      </c>
+      <c r="G54">
+        <v>0.5</v>
+      </c>
+      <c r="H54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I54">
+        <v>5</v>
+      </c>
+      <c r="J54">
+        <v>4.92</v>
+      </c>
+      <c r="K54">
+        <v>2.5354627641843101E-2</v>
+      </c>
+      <c r="L54" t="s">
+        <v>56</v>
+      </c>
+      <c r="M54">
+        <v>0.14651376066498201</v>
+      </c>
+      <c r="N54">
+        <v>1.62754097761134E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FWHM data run for sg_rr_36_025 2023-12-13 16-41-08.csv
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B77C99-A6C8-4E95-87A8-517116D571FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759099E2-DC6A-4D67-BC08-32BAF3C40EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -615,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="76" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="76" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1407,6 +1407,50 @@
         <v>1.62754097761134E-2</v>
       </c>
     </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55">
+        <v>0.01</v>
+      </c>
+      <c r="C55">
+        <v>1000</v>
+      </c>
+      <c r="D55">
+        <v>5001</v>
+      </c>
+      <c r="E55">
+        <v>1530</v>
+      </c>
+      <c r="F55">
+        <v>1570</v>
+      </c>
+      <c r="G55">
+        <v>0.6</v>
+      </c>
+      <c r="H55" t="s">
+        <v>30</v>
+      </c>
+      <c r="I55">
+        <v>2.5</v>
+      </c>
+      <c r="J55">
+        <v>2.7278571428571401</v>
+      </c>
+      <c r="K55">
+        <v>1.3390933927838499E-2</v>
+      </c>
+      <c r="L55" t="s">
+        <v>56</v>
+      </c>
+      <c r="M55">
+        <v>0.146673785825335</v>
+      </c>
+      <c r="N55">
+        <v>5.4796550918534302E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FWHM data run for sg_rr_52_025 2023-12-11 18-30-06.
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759099E2-DC6A-4D67-BC08-32BAF3C40EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47641526-086C-4D84-A50F-6004311E7E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="74">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>peak data is found in same way as above although may adjust parameters like approx_fsr if see fit</t>
+  </si>
+  <si>
+    <t>reduced approx fsr a bit, to see if this had any affect on fsr calculation as above, half the approx fsr was quite close to actual calculated fsr.</t>
   </si>
 </sst>
 </file>
@@ -615,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="76" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="73" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1314,12 +1317,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -1363,7 +1366,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -1407,7 +1410,7 @@
         <v>1.62754097761134E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -1449,6 +1452,53 @@
       </c>
       <c r="N55">
         <v>5.4796550918534302E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56">
+        <v>0.01</v>
+      </c>
+      <c r="C56">
+        <v>1000</v>
+      </c>
+      <c r="D56">
+        <v>5001</v>
+      </c>
+      <c r="E56">
+        <v>1530</v>
+      </c>
+      <c r="F56">
+        <v>1570</v>
+      </c>
+      <c r="G56">
+        <v>0.5</v>
+      </c>
+      <c r="H56" t="s">
+        <v>30</v>
+      </c>
+      <c r="I56">
+        <v>2</v>
+      </c>
+      <c r="J56">
+        <v>1.8875</v>
+      </c>
+      <c r="K56">
+        <v>7.8430324425366096E-3</v>
+      </c>
+      <c r="L56" t="s">
+        <v>56</v>
+      </c>
+      <c r="M56">
+        <v>0.140490273155437</v>
+      </c>
+      <c r="N56">
+        <v>6.6112105211042198E-3</v>
+      </c>
+      <c r="O56" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FWHM data run for sg_rr_68_025 2023-12-11 17-15-27
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47641526-086C-4D84-A50F-6004311E7E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F35500-A963-4123-A8CF-AD847F52669F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>reduced approx fsr a bit, to see if this had any affect on fsr calculation as above, half the approx fsr was quite close to actual calculated fsr.</t>
+  </si>
+  <si>
+    <t>yes (although start peak maybe missed)</t>
   </si>
 </sst>
 </file>
@@ -618,9 +621,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:O56"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="73" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="73" workbookViewId="0">
       <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
@@ -637,7 +640,7 @@
     <col min="9" max="9" width="14.08984375" customWidth="1"/>
     <col min="10" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
     <col min="13" max="13" width="15.36328125" customWidth="1"/>
     <col min="14" max="14" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1501,6 +1504,50 @@
         <v>73</v>
       </c>
     </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>40</v>
+      </c>
+      <c r="B57">
+        <v>0.01</v>
+      </c>
+      <c r="C57">
+        <v>1000</v>
+      </c>
+      <c r="D57">
+        <v>5001</v>
+      </c>
+      <c r="E57">
+        <v>1530</v>
+      </c>
+      <c r="F57">
+        <v>1570</v>
+      </c>
+      <c r="G57">
+        <v>0.5</v>
+      </c>
+      <c r="H57" t="s">
+        <v>30</v>
+      </c>
+      <c r="I57">
+        <v>1.7</v>
+      </c>
+      <c r="J57">
+        <v>1.4480769230769099</v>
+      </c>
+      <c r="K57">
+        <v>6.22696940163916E-3</v>
+      </c>
+      <c r="L57" t="s">
+        <v>74</v>
+      </c>
+      <c r="M57">
+        <v>0.137531855376269</v>
+      </c>
+      <c r="N57">
+        <v>2.0576576158408901E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FWHM data run for sg_rr_84_025 2023-12-11 16-27-03
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F35500-A963-4123-A8CF-AD847F52669F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A8EAD5-82F3-4C5A-9049-D8AD8D854B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -621,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="73" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="73" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1548,6 +1548,50 @@
         <v>2.0576576158408901E-3</v>
       </c>
     </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>45</v>
+      </c>
+      <c r="B58">
+        <v>0.01</v>
+      </c>
+      <c r="C58">
+        <v>1000</v>
+      </c>
+      <c r="D58">
+        <v>5001</v>
+      </c>
+      <c r="E58">
+        <v>1530</v>
+      </c>
+      <c r="F58">
+        <v>1570</v>
+      </c>
+      <c r="G58">
+        <v>0.5</v>
+      </c>
+      <c r="H58" t="s">
+        <v>30</v>
+      </c>
+      <c r="I58">
+        <v>1.7</v>
+      </c>
+      <c r="J58">
+        <v>1.1724242424242399</v>
+      </c>
+      <c r="K58">
+        <v>5.9834098769671303E-3</v>
+      </c>
+      <c r="L58" t="s">
+        <v>56</v>
+      </c>
+      <c r="M58">
+        <v>0.139397560714696</v>
+      </c>
+      <c r="N58">
+        <v>5.4333187796293501E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FWHM data run for sg_rr_100_025 2023-12-11 14-23-14
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A8EAD5-82F3-4C5A-9049-D8AD8D854B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491E0B6C-16DC-4380-B03E-AC90AF2E5756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>yes (although start peak maybe missed)</t>
+  </si>
+  <si>
+    <t>yes(although possible end peak not found)</t>
   </si>
 </sst>
 </file>
@@ -621,9 +624,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="73" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="73" workbookViewId="0">
       <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
@@ -1592,6 +1595,53 @@
         <v>5.4333187796293501E-3</v>
       </c>
     </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59">
+        <v>0.01</v>
+      </c>
+      <c r="C59">
+        <v>1000</v>
+      </c>
+      <c r="D59">
+        <v>5001</v>
+      </c>
+      <c r="E59">
+        <v>1530</v>
+      </c>
+      <c r="F59">
+        <v>1570</v>
+      </c>
+      <c r="G59">
+        <v>0.5</v>
+      </c>
+      <c r="H59" t="s">
+        <v>30</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>0.98282051282051597</v>
+      </c>
+      <c r="K59">
+        <v>5.5097596875867197E-3</v>
+      </c>
+      <c r="L59" t="s">
+        <v>75</v>
+      </c>
+      <c r="M59">
+        <v>0.14513350341842499</v>
+      </c>
+      <c r="N59">
+        <v>3.6926757851065001E-3</v>
+      </c>
+      <c r="O59" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FWHM data run for sg_rr_100_027 2023-12-08 17-44-55.csv
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491E0B6C-16DC-4380-B03E-AC90AF2E5756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855604B4-8CBE-4558-9BE8-88BF28DC5C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -624,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="73" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="73" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1642,6 +1642,53 @@
         <v>73</v>
       </c>
     </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>51</v>
+      </c>
+      <c r="B60">
+        <v>0.01</v>
+      </c>
+      <c r="C60">
+        <v>1000</v>
+      </c>
+      <c r="D60">
+        <v>5001</v>
+      </c>
+      <c r="E60">
+        <v>1530</v>
+      </c>
+      <c r="F60">
+        <v>1570</v>
+      </c>
+      <c r="G60">
+        <v>0.5</v>
+      </c>
+      <c r="H60" t="s">
+        <v>30</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>0.98153846153846003</v>
+      </c>
+      <c r="K60">
+        <v>4.3858818636388196E-3</v>
+      </c>
+      <c r="L60" t="s">
+        <v>75</v>
+      </c>
+      <c r="M60">
+        <v>0.126322698170279</v>
+      </c>
+      <c r="N60">
+        <v>3.2111503732971001E-3</v>
+      </c>
+      <c r="O60" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FWHM data run for sg_rr_100_028 2023-12-08 16-58-05
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855604B4-8CBE-4558-9BE8-88BF28DC5C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20A8B83-F738-4E22-90F7-BB877FB98AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="76">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -624,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="73" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="73" workbookViewId="0">
+      <selection activeCell="O60" sqref="O60:O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1689,6 +1689,53 @@
         <v>73</v>
       </c>
     </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B61">
+        <v>0.01</v>
+      </c>
+      <c r="C61">
+        <v>1000</v>
+      </c>
+      <c r="D61">
+        <v>5001</v>
+      </c>
+      <c r="E61">
+        <v>1530</v>
+      </c>
+      <c r="F61">
+        <v>1570</v>
+      </c>
+      <c r="G61">
+        <v>0.5</v>
+      </c>
+      <c r="H61" t="s">
+        <v>30</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>0.98274999999999801</v>
+      </c>
+      <c r="K61">
+        <v>3.2814064370514399E-3</v>
+      </c>
+      <c r="L61" t="s">
+        <v>56</v>
+      </c>
+      <c r="M61">
+        <v>0.102827046790518</v>
+      </c>
+      <c r="N61">
+        <v>2.13794013833199E-3</v>
+      </c>
+      <c r="O61" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FWHM data run for sg_rr_100_030 2023-12-08 16-08-32
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20A8B83-F738-4E22-90F7-BB877FB98AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86434BA-932C-4A3D-BD16-DAEC65DEF18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="76">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -624,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="73" workbookViewId="0">
-      <selection activeCell="O60" sqref="O60:O61"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="73" workbookViewId="0">
+      <selection activeCell="N62" sqref="N62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1736,6 +1736,50 @@
         <v>73</v>
       </c>
     </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62">
+        <v>0.01</v>
+      </c>
+      <c r="C62">
+        <v>1000</v>
+      </c>
+      <c r="D62">
+        <v>5001</v>
+      </c>
+      <c r="E62">
+        <v>1530</v>
+      </c>
+      <c r="F62">
+        <v>1570</v>
+      </c>
+      <c r="G62">
+        <v>0.5</v>
+      </c>
+      <c r="H62" t="s">
+        <v>30</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>0.98128205128205004</v>
+      </c>
+      <c r="K62">
+        <v>3.16397329552258E-3</v>
+      </c>
+      <c r="L62" t="s">
+        <v>56</v>
+      </c>
+      <c r="M62">
+        <v>7.8026629228047706E-2</v>
+      </c>
+      <c r="N62">
+        <v>1.9636937441561801E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
setting up table for collecting Q factor data
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86434BA-932C-4A3D-BD16-DAEC65DEF18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393CF06A-E50E-4283-A1D6-5DCD78B3A0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="88">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -264,6 +264,42 @@
   </si>
   <si>
     <t>yes(although possible end peak not found)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The analysis results below will calculate fsr and fwhm data from the saved wavelength sweep data, in a similar way to above. </t>
+  </si>
+  <si>
+    <t>The difference however, is that to find the peaks and their FWHM, I have converted powers first into mW from dBm.</t>
+  </si>
+  <si>
+    <t>The rest is as above, and can refer to the notebook saved in the same directory as the one used above, but is this time called: data_analysis_notebook_Q_factor.</t>
+  </si>
+  <si>
+    <t>In addition to calculating the above. The notebook finds a list of Q factors by taking each peak_wavelengths/peak FWHM. And finds the mean Q factor and standard error in the Q factor in the same way the mean and standard error for the fsr are found from the list of fsrs.</t>
+  </si>
+  <si>
+    <t>Also, when I input the ring radius, and its error. The notebook calculates Q^3/R^2 and its associated uncertainty as well.</t>
+  </si>
+  <si>
+    <t>Also, note this time, I'll choose the prominence and it will be in mW.</t>
+  </si>
+  <si>
+    <t>prominence/mW</t>
+  </si>
+  <si>
+    <t>I will choose the prominence roughly by looking at height span of roughly biggest height span noise. But it is very rough, and main check is whether code visually appears to find peaks.</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Q error</t>
+  </si>
+  <si>
+    <t>Q^3/R^2 (micrometres^-2)</t>
+  </si>
+  <si>
+    <t>Q^3/R^2 error (micrometres^-2)</t>
   </si>
 </sst>
 </file>
@@ -624,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:O62"/>
+  <dimension ref="A1:R73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="73" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="73" workbookViewId="0">
+      <selection activeCell="R72" sqref="R72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1780,6 +1816,102 @@
         <v>1.9636937441561801E-3</v>
       </c>
     </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>66</v>
+      </c>
+      <c r="B72" t="s">
+        <v>23</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>2</v>
+      </c>
+      <c r="E72" t="s">
+        <v>24</v>
+      </c>
+      <c r="F72" t="s">
+        <v>25</v>
+      </c>
+      <c r="G72" t="s">
+        <v>82</v>
+      </c>
+      <c r="H72" t="s">
+        <v>3</v>
+      </c>
+      <c r="I72" t="s">
+        <v>26</v>
+      </c>
+      <c r="J72" t="s">
+        <v>27</v>
+      </c>
+      <c r="K72" t="s">
+        <v>28</v>
+      </c>
+      <c r="L72" t="s">
+        <v>43</v>
+      </c>
+      <c r="M72" t="s">
+        <v>68</v>
+      </c>
+      <c r="N72" t="s">
+        <v>67</v>
+      </c>
+      <c r="O72" t="s">
+        <v>84</v>
+      </c>
+      <c r="P72" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>86</v>
+      </c>
+      <c r="R72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="H73" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Q factor run for sg_rr_20_025 2023-12-13 17-59-26.csv data
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393CF06A-E50E-4283-A1D6-5DCD78B3A0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244D855D-D7D0-40F9-8FFB-8E7158774FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="92">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -287,9 +287,6 @@
     <t>prominence/mW</t>
   </si>
   <si>
-    <t>I will choose the prominence roughly by looking at height span of roughly biggest height span noise. But it is very rough, and main check is whether code visually appears to find peaks.</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -300,6 +297,21 @@
   </si>
   <si>
     <t>Q^3/R^2 error (micrometres^-2)</t>
+  </si>
+  <si>
+    <t>I will choose the prominence roughly by looking at height span of roughly biggest height span noise. But it is very rough, and main check is whether code visually appears to find peaks. I may actually make the prominence a bit less that full height span of biggest height span on noise depending on how high the peaks seem to be above the noise. I will try and see what I can get away with.</t>
+  </si>
+  <si>
+    <t>I will use same approx fsrs as above.</t>
+  </si>
+  <si>
+    <t>radis/micrometres</t>
+  </si>
+  <si>
+    <t>radius error/ micrometres</t>
+  </si>
+  <si>
+    <t>I get the radius from the filename, and assume the error for all to be 0.1 micrometres.</t>
   </si>
 </sst>
 </file>
@@ -660,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:R73"/>
+  <dimension ref="A1:T75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="73" workbookViewId="0">
-      <selection activeCell="R72" sqref="R72"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="73" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1821,95 +1833,168 @@
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" t="s">
+        <v>23</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
+        <v>2</v>
+      </c>
+      <c r="E74" t="s">
+        <v>24</v>
+      </c>
+      <c r="F74" t="s">
+        <v>25</v>
+      </c>
+      <c r="G74" t="s">
+        <v>82</v>
+      </c>
+      <c r="H74" t="s">
+        <v>3</v>
+      </c>
+      <c r="I74" t="s">
+        <v>26</v>
+      </c>
+      <c r="J74" t="s">
+        <v>27</v>
+      </c>
+      <c r="K74" t="s">
+        <v>28</v>
+      </c>
+      <c r="L74" t="s">
+        <v>43</v>
+      </c>
+      <c r="M74" t="s">
+        <v>68</v>
+      </c>
+      <c r="N74" t="s">
+        <v>67</v>
+      </c>
+      <c r="O74" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>66</v>
-      </c>
-      <c r="B72" t="s">
-        <v>23</v>
-      </c>
-      <c r="C72" t="s">
-        <v>1</v>
-      </c>
-      <c r="D72" t="s">
-        <v>2</v>
-      </c>
-      <c r="E72" t="s">
-        <v>24</v>
-      </c>
-      <c r="F72" t="s">
-        <v>25</v>
-      </c>
-      <c r="G72" t="s">
-        <v>82</v>
-      </c>
-      <c r="H72" t="s">
-        <v>3</v>
-      </c>
-      <c r="I72" t="s">
-        <v>26</v>
-      </c>
-      <c r="J72" t="s">
-        <v>27</v>
-      </c>
-      <c r="K72" t="s">
-        <v>28</v>
-      </c>
-      <c r="L72" t="s">
-        <v>43</v>
-      </c>
-      <c r="M72" t="s">
-        <v>68</v>
-      </c>
-      <c r="N72" t="s">
-        <v>67</v>
-      </c>
-      <c r="O72" t="s">
+      <c r="P74" t="s">
         <v>84</v>
       </c>
-      <c r="P72" t="s">
+      <c r="Q74" t="s">
         <v>85</v>
       </c>
-      <c r="Q72" t="s">
+      <c r="R74" t="s">
         <v>86</v>
       </c>
-      <c r="R72" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="H73" t="s">
+      <c r="S74" t="s">
+        <v>89</v>
+      </c>
+      <c r="T74" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75">
+        <v>0.01</v>
+      </c>
+      <c r="C75">
+        <v>1000</v>
+      </c>
+      <c r="D75">
+        <v>5001</v>
+      </c>
+      <c r="E75">
+        <v>1530</v>
+      </c>
+      <c r="F75">
+        <v>1570</v>
+      </c>
+      <c r="G75">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H75" t="s">
         <v>30</v>
+      </c>
+      <c r="I75">
+        <v>5</v>
+      </c>
+      <c r="J75">
+        <v>4.92</v>
+      </c>
+      <c r="K75">
+        <v>2.5354627641843101E-2</v>
+      </c>
+      <c r="L75" t="s">
+        <v>56</v>
+      </c>
+      <c r="M75">
+        <v>0.15234521434913001</v>
+      </c>
+      <c r="N75">
+        <v>1.60120635742305E-2</v>
+      </c>
+      <c r="O75">
+        <v>11059.505619039001</v>
+      </c>
+      <c r="P75">
+        <v>1285.5192974044101</v>
+      </c>
+      <c r="Q75">
+        <v>3381794001.8318701</v>
+      </c>
+      <c r="R75">
+        <v>1179749480.62256</v>
+      </c>
+      <c r="S75">
+        <v>20</v>
+      </c>
+      <c r="T75">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Q factor run for sg_rr_36_025 2023-12-13 16-41-08.csv that seems to have gone wrong
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244D855D-D7D0-40F9-8FFB-8E7158774FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684C02F4-B006-4A6B-8D16-4F43B75A88B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="95">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>I get the radius from the filename, and assume the error for all to be 0.1 micrometres.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actually for highlighted yellow run below, I chose prominence to be roughly full height span of biggest height span noise. But I realise above, that I chose it to be around half the height span of the noise, so I will continue to do this for the rest of the data runs. </t>
+  </si>
+  <si>
+    <t>didn't double count peaks, but seemed to find peaks in noise, so wrong anyway.</t>
+  </si>
+  <si>
+    <t>looks like prominence was probably too low as seems visually to find peaks in noise, going to try increasing it.</t>
   </si>
 </sst>
 </file>
@@ -332,12 +341,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -352,12 +367,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:T75"/>
+  <dimension ref="A1:U77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="73" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="73" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1833,168 +1849,238 @@
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>66</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>23</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>1</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D75" t="s">
         <v>2</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E75" t="s">
         <v>24</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F75" t="s">
         <v>25</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G75" t="s">
         <v>82</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H75" t="s">
         <v>3</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I75" t="s">
         <v>26</v>
       </c>
-      <c r="J74" t="s">
+      <c r="J75" t="s">
         <v>27</v>
       </c>
-      <c r="K74" t="s">
+      <c r="K75" t="s">
         <v>28</v>
       </c>
-      <c r="L74" t="s">
+      <c r="L75" t="s">
         <v>43</v>
       </c>
-      <c r="M74" t="s">
+      <c r="M75" t="s">
         <v>68</v>
       </c>
-      <c r="N74" t="s">
+      <c r="N75" t="s">
         <v>67</v>
       </c>
-      <c r="O74" t="s">
+      <c r="O75" t="s">
         <v>83</v>
       </c>
-      <c r="P74" t="s">
+      <c r="P75" t="s">
         <v>84</v>
       </c>
-      <c r="Q74" t="s">
+      <c r="Q75" t="s">
         <v>85</v>
       </c>
-      <c r="R74" t="s">
+      <c r="R75" t="s">
         <v>86</v>
       </c>
-      <c r="S74" t="s">
+      <c r="S75" t="s">
         <v>89</v>
       </c>
-      <c r="T74" t="s">
+      <c r="T75" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B75">
-        <v>0.01</v>
-      </c>
-      <c r="C75">
-        <v>1000</v>
-      </c>
-      <c r="D75">
-        <v>5001</v>
-      </c>
-      <c r="E75">
-        <v>1530</v>
-      </c>
-      <c r="F75">
-        <v>1570</v>
-      </c>
-      <c r="G75">
+      <c r="B76" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C76" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D76" s="3">
+        <v>5001</v>
+      </c>
+      <c r="E76" s="3">
+        <v>1530</v>
+      </c>
+      <c r="F76" s="3">
+        <v>1570</v>
+      </c>
+      <c r="G76" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H75" t="s">
-        <v>30</v>
-      </c>
-      <c r="I75">
+      <c r="H76" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I76" s="3">
         <v>5</v>
       </c>
-      <c r="J75">
+      <c r="J76" s="3">
         <v>4.92</v>
       </c>
-      <c r="K75">
+      <c r="K76" s="3">
         <v>2.5354627641843101E-2</v>
       </c>
-      <c r="L75" t="s">
+      <c r="L76" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="M75">
+      <c r="M76" s="3">
         <v>0.15234521434913001</v>
       </c>
-      <c r="N75">
+      <c r="N76" s="3">
         <v>1.60120635742305E-2</v>
       </c>
-      <c r="O75">
+      <c r="O76" s="3">
         <v>11059.505619039001</v>
       </c>
-      <c r="P75">
+      <c r="P76" s="3">
         <v>1285.5192974044101</v>
       </c>
-      <c r="Q75">
+      <c r="Q76" s="3">
         <v>3381794001.8318701</v>
       </c>
-      <c r="R75">
+      <c r="R76" s="3">
         <v>1179749480.62256</v>
       </c>
-      <c r="S75">
+      <c r="S76" s="3">
         <v>20</v>
       </c>
-      <c r="T75">
+      <c r="T76" s="3">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>36</v>
+      </c>
+      <c r="B77">
+        <v>0.01</v>
+      </c>
+      <c r="C77">
+        <v>1000</v>
+      </c>
+      <c r="D77">
+        <v>5001</v>
+      </c>
+      <c r="E77">
+        <v>1530</v>
+      </c>
+      <c r="F77">
+        <v>1570</v>
+      </c>
+      <c r="G77">
+        <v>0.01</v>
+      </c>
+      <c r="H77" t="s">
+        <v>30</v>
+      </c>
+      <c r="I77">
+        <v>2.5</v>
+      </c>
+      <c r="J77">
+        <v>1.41444444444444</v>
+      </c>
+      <c r="K77">
+        <v>4.8543848458607999E-2</v>
+      </c>
+      <c r="L77" t="s">
+        <v>93</v>
+      </c>
+      <c r="M77">
+        <v>0.13344435261279899</v>
+      </c>
+      <c r="N77">
+        <v>6.1168450977610901E-3</v>
+      </c>
+      <c r="O77">
+        <v>12194.6355018502</v>
+      </c>
+      <c r="P77">
+        <v>476.89194268563199</v>
+      </c>
+      <c r="Q77">
+        <v>1399269828.2413299</v>
+      </c>
+      <c r="R77">
+        <v>164346427.56564301</v>
+      </c>
+      <c r="S77">
+        <v>36</v>
+      </c>
+      <c r="T77">
+        <v>0.1</v>
+      </c>
+      <c r="U77" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Q factor data run for sg_rr_36_025 2023-12-13 16-41-08.csv
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684C02F4-B006-4A6B-8D16-4F43B75A88B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B71130-ED50-486A-8829-6104057E810A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="96">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>looks like prominence was probably too low as seems visually to find peaks in noise, going to try increasing it.</t>
+  </si>
+  <si>
+    <t>looks like prominence was probably too low as seems visually to find peaks in noise, going to try increasing it again without recording rest of data.</t>
   </si>
 </sst>
 </file>
@@ -688,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:U77"/>
+  <dimension ref="A1:V81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="73" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="73" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1849,238 +1852,370 @@
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>66</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>23</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>1</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>2</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E76" t="s">
         <v>24</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F76" t="s">
         <v>25</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G76" t="s">
         <v>82</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H76" t="s">
         <v>3</v>
       </c>
-      <c r="I75" t="s">
+      <c r="I76" t="s">
         <v>26</v>
       </c>
-      <c r="J75" t="s">
+      <c r="J76" t="s">
         <v>27</v>
       </c>
-      <c r="K75" t="s">
+      <c r="K76" t="s">
         <v>28</v>
       </c>
-      <c r="L75" t="s">
+      <c r="L76" t="s">
         <v>43</v>
       </c>
-      <c r="M75" t="s">
+      <c r="M76" t="s">
         <v>68</v>
       </c>
-      <c r="N75" t="s">
+      <c r="N76" t="s">
         <v>67</v>
       </c>
-      <c r="O75" t="s">
+      <c r="O76" t="s">
         <v>83</v>
       </c>
-      <c r="P75" t="s">
+      <c r="P76" t="s">
         <v>84</v>
       </c>
-      <c r="Q75" t="s">
+      <c r="Q76" t="s">
         <v>85</v>
       </c>
-      <c r="R75" t="s">
+      <c r="R76" t="s">
         <v>86</v>
       </c>
-      <c r="S75" t="s">
+      <c r="S76" t="s">
         <v>89</v>
       </c>
-      <c r="T75" t="s">
+      <c r="T76" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A76" s="3" t="s">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B76" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="C76" s="3">
-        <v>1000</v>
-      </c>
-      <c r="D76" s="3">
-        <v>5001</v>
-      </c>
-      <c r="E76" s="3">
-        <v>1530</v>
-      </c>
-      <c r="F76" s="3">
-        <v>1570</v>
-      </c>
-      <c r="G76" s="3">
+      <c r="B77" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C77" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D77" s="3">
+        <v>5001</v>
+      </c>
+      <c r="E77" s="3">
+        <v>1530</v>
+      </c>
+      <c r="F77" s="3">
+        <v>1570</v>
+      </c>
+      <c r="G77" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H76" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" s="3">
+      <c r="H77" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I77" s="3">
         <v>5</v>
       </c>
-      <c r="J76" s="3">
+      <c r="J77" s="3">
         <v>4.92</v>
       </c>
-      <c r="K76" s="3">
+      <c r="K77" s="3">
         <v>2.5354627641843101E-2</v>
       </c>
-      <c r="L76" s="3" t="s">
+      <c r="L77" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="M76" s="3">
+      <c r="M77" s="3">
         <v>0.15234521434913001</v>
       </c>
-      <c r="N76" s="3">
+      <c r="N77" s="3">
         <v>1.60120635742305E-2</v>
       </c>
-      <c r="O76" s="3">
+      <c r="O77" s="3">
         <v>11059.505619039001</v>
       </c>
-      <c r="P76" s="3">
+      <c r="P77" s="3">
         <v>1285.5192974044101</v>
       </c>
-      <c r="Q76" s="3">
+      <c r="Q77" s="3">
         <v>3381794001.8318701</v>
       </c>
-      <c r="R76" s="3">
+      <c r="R77" s="3">
         <v>1179749480.62256</v>
       </c>
-      <c r="S76" s="3">
+      <c r="S77" s="3">
         <v>20</v>
       </c>
-      <c r="T76" s="3">
+      <c r="T77" s="3">
         <v>0.1</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>36</v>
       </c>
-      <c r="B77">
-        <v>0.01</v>
-      </c>
-      <c r="C77">
-        <v>1000</v>
-      </c>
-      <c r="D77">
-        <v>5001</v>
-      </c>
-      <c r="E77">
-        <v>1530</v>
-      </c>
-      <c r="F77">
-        <v>1570</v>
-      </c>
-      <c r="G77">
-        <v>0.01</v>
-      </c>
-      <c r="H77" t="s">
-        <v>30</v>
-      </c>
-      <c r="I77">
+      <c r="B78">
+        <v>0.01</v>
+      </c>
+      <c r="C78">
+        <v>1000</v>
+      </c>
+      <c r="D78">
+        <v>5001</v>
+      </c>
+      <c r="E78">
+        <v>1530</v>
+      </c>
+      <c r="F78">
+        <v>1570</v>
+      </c>
+      <c r="G78">
+        <v>0.01</v>
+      </c>
+      <c r="H78" t="s">
+        <v>30</v>
+      </c>
+      <c r="I78">
         <v>2.5</v>
       </c>
-      <c r="J77">
+      <c r="J78">
         <v>1.41444444444444</v>
       </c>
-      <c r="K77">
+      <c r="K78">
         <v>4.8543848458607999E-2</v>
       </c>
-      <c r="L77" t="s">
+      <c r="L78" t="s">
         <v>93</v>
       </c>
-      <c r="M77">
+      <c r="M78">
         <v>0.13344435261279899</v>
       </c>
-      <c r="N77">
+      <c r="N78">
         <v>6.1168450977610901E-3</v>
       </c>
-      <c r="O77">
+      <c r="O78">
         <v>12194.6355018502</v>
       </c>
-      <c r="P77">
+      <c r="P78">
         <v>476.89194268563199</v>
       </c>
-      <c r="Q77">
+      <c r="Q78">
         <v>1399269828.2413299</v>
       </c>
-      <c r="R77">
+      <c r="R78">
         <v>164346427.56564301</v>
       </c>
-      <c r="S77">
+      <c r="S78">
         <v>36</v>
       </c>
-      <c r="T77">
+      <c r="T78">
         <v>0.1</v>
       </c>
-      <c r="U77" t="s">
+      <c r="U78" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>36</v>
+      </c>
+      <c r="B79">
+        <v>0.01</v>
+      </c>
+      <c r="C79">
+        <v>1000</v>
+      </c>
+      <c r="D79">
+        <v>5001</v>
+      </c>
+      <c r="E79">
+        <v>1530</v>
+      </c>
+      <c r="F79">
+        <v>1570</v>
+      </c>
+      <c r="G79">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H79" t="s">
+        <v>30</v>
+      </c>
+      <c r="I79">
+        <v>2.5</v>
+      </c>
+      <c r="U79" t="s">
+        <v>95</v>
+      </c>
+      <c r="V79" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>36</v>
+      </c>
+      <c r="B80">
+        <v>0.01</v>
+      </c>
+      <c r="C80">
+        <v>1000</v>
+      </c>
+      <c r="D80">
+        <v>5001</v>
+      </c>
+      <c r="E80">
+        <v>1530</v>
+      </c>
+      <c r="F80">
+        <v>1570</v>
+      </c>
+      <c r="G80">
+        <v>0.02</v>
+      </c>
+      <c r="H80" t="s">
+        <v>30</v>
+      </c>
+      <c r="I80">
+        <v>2.5</v>
+      </c>
+      <c r="U80" t="s">
+        <v>95</v>
+      </c>
+      <c r="V80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>36</v>
+      </c>
+      <c r="B81">
+        <v>0.01</v>
+      </c>
+      <c r="C81">
+        <v>1000</v>
+      </c>
+      <c r="D81">
+        <v>5001</v>
+      </c>
+      <c r="E81">
+        <v>1530</v>
+      </c>
+      <c r="F81">
+        <v>1570</v>
+      </c>
+      <c r="G81">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="H81" t="s">
+        <v>30</v>
+      </c>
+      <c r="I81">
+        <v>2.5</v>
+      </c>
+      <c r="J81">
+        <v>2.7278571428571401</v>
+      </c>
+      <c r="K81">
+        <v>1.3390933927838499E-2</v>
+      </c>
+      <c r="L81" t="s">
+        <v>56</v>
+      </c>
+      <c r="M81">
+        <v>0.15637520677942199</v>
+      </c>
+      <c r="N81">
+        <v>7.2204120216507297E-3</v>
+      </c>
+      <c r="O81">
+        <v>10163.830903419301</v>
+      </c>
+      <c r="P81">
+        <v>389.61853012136697</v>
+      </c>
+      <c r="Q81">
+        <v>810153460.86979795</v>
+      </c>
+      <c r="R81">
+        <v>93277498.042337507</v>
+      </c>
+      <c r="S81">
+        <v>36</v>
+      </c>
+      <c r="T81">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Q factor data run for sg_rr_52_025 2023-12-11 18-30-06.csv data
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B71130-ED50-486A-8829-6104057E810A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AE5E16-B60E-4EC4-ADBF-C0E26CA60D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="96">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -691,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:V81"/>
+  <dimension ref="A1:V82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="73" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="73" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2218,6 +2218,68 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82">
+        <v>0.01</v>
+      </c>
+      <c r="C82">
+        <v>1000</v>
+      </c>
+      <c r="D82">
+        <v>5001</v>
+      </c>
+      <c r="E82">
+        <v>1530</v>
+      </c>
+      <c r="F82">
+        <v>1570</v>
+      </c>
+      <c r="G82">
+        <v>0.01</v>
+      </c>
+      <c r="H82" t="s">
+        <v>30</v>
+      </c>
+      <c r="I82">
+        <v>2</v>
+      </c>
+      <c r="J82">
+        <v>1.8875</v>
+      </c>
+      <c r="K82">
+        <v>7.8430324425366096E-3</v>
+      </c>
+      <c r="L82" t="s">
+        <v>56</v>
+      </c>
+      <c r="M82">
+        <v>0.151131672031217</v>
+      </c>
+      <c r="N82">
+        <v>6.0602112450080696E-3</v>
+      </c>
+      <c r="O82">
+        <v>10509.3396239214</v>
+      </c>
+      <c r="P82">
+        <v>323.17436740347603</v>
+      </c>
+      <c r="Q82">
+        <v>895614837.28920305</v>
+      </c>
+      <c r="R82">
+        <v>82773263.426702306</v>
+      </c>
+      <c r="S82">
+        <v>52</v>
+      </c>
+      <c r="T82">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Q factor data run for sg_rr_68_025 2023-12-11 17-15-27.csv
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AE5E16-B60E-4EC4-ADBF-C0E26CA60D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85422599-CAA4-4D4D-BF73-A43E3089A41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="98">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>looks like prominence was probably too low as seems visually to find peaks in noise, going to try increasing it again without recording rest of data.</t>
+  </si>
+  <si>
+    <t>found one peak in what looked like noise at end, so increased prominence slightly</t>
+  </si>
+  <si>
+    <t>yes, although  maybe misses peak at start which may be cut off in range</t>
   </si>
 </sst>
 </file>
@@ -691,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:V82"/>
+  <dimension ref="A1:V84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="73" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="105" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2156,7 +2162,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>36</v>
       </c>
@@ -2218,7 +2224,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>38</v>
       </c>
@@ -2277,6 +2283,100 @@
         <v>52</v>
       </c>
       <c r="T82">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>40</v>
+      </c>
+      <c r="B83">
+        <v>0.01</v>
+      </c>
+      <c r="C83">
+        <v>1000</v>
+      </c>
+      <c r="D83">
+        <v>5001</v>
+      </c>
+      <c r="E83">
+        <v>1530</v>
+      </c>
+      <c r="F83">
+        <v>1570</v>
+      </c>
+      <c r="G83">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H83" t="s">
+        <v>30</v>
+      </c>
+      <c r="I83">
+        <v>1.7</v>
+      </c>
+      <c r="U83" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>40</v>
+      </c>
+      <c r="B84">
+        <v>0.01</v>
+      </c>
+      <c r="C84">
+        <v>1000</v>
+      </c>
+      <c r="D84">
+        <v>5001</v>
+      </c>
+      <c r="E84">
+        <v>1530</v>
+      </c>
+      <c r="F84">
+        <v>1570</v>
+      </c>
+      <c r="G84">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H84" t="s">
+        <v>30</v>
+      </c>
+      <c r="I84">
+        <v>1.7</v>
+      </c>
+      <c r="J84">
+        <v>1.4480769230769099</v>
+      </c>
+      <c r="K84">
+        <v>6.22696940163916E-3</v>
+      </c>
+      <c r="L84" t="s">
+        <v>97</v>
+      </c>
+      <c r="M84">
+        <v>0.14551002990475601</v>
+      </c>
+      <c r="N84">
+        <v>4.0795003221365698E-3</v>
+      </c>
+      <c r="O84">
+        <v>10813.9579876443</v>
+      </c>
+      <c r="P84">
+        <v>225.45654915634299</v>
+      </c>
+      <c r="Q84">
+        <v>273486698.55092198</v>
+      </c>
+      <c r="R84">
+        <v>17124396.8345199</v>
+      </c>
+      <c r="S84">
+        <v>68</v>
+      </c>
+      <c r="T84">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Q factor run for sg_rr_84_025 2023-12-11 16-27-03.csv data
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85422599-CAA4-4D4D-BF73-A43E3089A41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1426D5BB-4F5C-42B8-AE6F-253946E417C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="100">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -330,6 +330,12 @@
   </si>
   <si>
     <t>yes, although  maybe misses peak at start which may be cut off in range</t>
+  </si>
+  <si>
+    <t>Note I mostly only committed to Git after each run that I thought had gone correctly after adjusting prominences.</t>
+  </si>
+  <si>
+    <t>seemed to find one peak in what looked like noise so increased prominence</t>
   </si>
 </sst>
 </file>
@@ -697,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:V84"/>
+  <dimension ref="A1:V87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="105" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="105" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1903,6 +1909,11 @@
         <v>91</v>
       </c>
     </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>98</v>
+      </c>
+    </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>66</v>
@@ -2377,6 +2388,132 @@
         <v>68</v>
       </c>
       <c r="T84">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>45</v>
+      </c>
+      <c r="B85">
+        <v>0.01</v>
+      </c>
+      <c r="C85">
+        <v>1000</v>
+      </c>
+      <c r="D85">
+        <v>5001</v>
+      </c>
+      <c r="E85">
+        <v>1530</v>
+      </c>
+      <c r="F85">
+        <v>1570</v>
+      </c>
+      <c r="G85">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="H85" t="s">
+        <v>30</v>
+      </c>
+      <c r="I85">
+        <v>1.7</v>
+      </c>
+      <c r="U85" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>45</v>
+      </c>
+      <c r="B86">
+        <v>0.01</v>
+      </c>
+      <c r="C86">
+        <v>1000</v>
+      </c>
+      <c r="D86">
+        <v>5001</v>
+      </c>
+      <c r="E86">
+        <v>1530</v>
+      </c>
+      <c r="F86">
+        <v>1570</v>
+      </c>
+      <c r="G86">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="H86" t="s">
+        <v>30</v>
+      </c>
+      <c r="I86">
+        <v>1.7</v>
+      </c>
+      <c r="U86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>45</v>
+      </c>
+      <c r="B87">
+        <v>0.01</v>
+      </c>
+      <c r="C87">
+        <v>1000</v>
+      </c>
+      <c r="D87">
+        <v>5001</v>
+      </c>
+      <c r="E87">
+        <v>1530</v>
+      </c>
+      <c r="F87">
+        <v>1570</v>
+      </c>
+      <c r="G87">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H87" t="s">
+        <v>30</v>
+      </c>
+      <c r="I87">
+        <v>1.7</v>
+      </c>
+      <c r="J87">
+        <v>1.1724242424242399</v>
+      </c>
+      <c r="K87">
+        <v>5.9834098769671303E-3</v>
+      </c>
+      <c r="L87" t="s">
+        <v>56</v>
+      </c>
+      <c r="M87">
+        <v>0.15082855204548801</v>
+      </c>
+      <c r="N87">
+        <v>5.8058346947930497E-3</v>
+      </c>
+      <c r="O87">
+        <v>10861.1687372212</v>
+      </c>
+      <c r="P87">
+        <v>523.81498314973601</v>
+      </c>
+      <c r="Q87">
+        <v>181581295.59314901</v>
+      </c>
+      <c r="R87">
+        <v>26275592.48443</v>
+      </c>
+      <c r="S87">
+        <v>84</v>
+      </c>
+      <c r="T87">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Q factor data run for sg_rr_100_025 2023-12-11 14-23-14
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1426D5BB-4F5C-42B8-AE6F-253946E417C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5990B7A1-AA78-4512-AE75-079061952266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="101">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>seemed to find one peak in what looked like noise so increased prominence</t>
+  </si>
+  <si>
+    <t>yes,although possible peak at end missed although hard to tell if it is a peak</t>
   </si>
 </sst>
 </file>
@@ -703,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:V87"/>
+  <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="105" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="105" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2517,6 +2520,68 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>48</v>
+      </c>
+      <c r="B88">
+        <v>0.01</v>
+      </c>
+      <c r="C88">
+        <v>1000</v>
+      </c>
+      <c r="D88">
+        <v>5001</v>
+      </c>
+      <c r="E88">
+        <v>1530</v>
+      </c>
+      <c r="F88">
+        <v>1570</v>
+      </c>
+      <c r="G88">
+        <v>1E-3</v>
+      </c>
+      <c r="H88" t="s">
+        <v>30</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>0.98282051282051597</v>
+      </c>
+      <c r="K88">
+        <v>5.5097596875867197E-3</v>
+      </c>
+      <c r="L88" t="s">
+        <v>100</v>
+      </c>
+      <c r="M88">
+        <v>0.16184922620443801</v>
+      </c>
+      <c r="N88">
+        <v>6.0009599444959304E-3</v>
+      </c>
+      <c r="O88">
+        <v>9978.8525564459196</v>
+      </c>
+      <c r="P88">
+        <v>283.12224613964702</v>
+      </c>
+      <c r="Q88">
+        <v>99366917.390740097</v>
+      </c>
+      <c r="R88">
+        <v>8460116.0168236997</v>
+      </c>
+      <c r="S88">
+        <v>100</v>
+      </c>
+      <c r="T88">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Q factor data run for sg_rr_100_027 2023-12-08 17-44-55
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5990B7A1-AA78-4512-AE75-079061952266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB8DA30-946D-4A3E-BB52-85A4F19A1F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="102">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>yes,although possible peak at end missed although hard to tell if it is a peak</t>
+  </si>
+  <si>
+    <t>actually have reason to think I recorded approx fsr wrong on this one, so need to redo. Because when putting in for next run saw it to still be 1.7.</t>
   </si>
 </sst>
 </file>
@@ -359,7 +362,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,6 +372,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,13 +394,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:V88"/>
+  <dimension ref="A1:V90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="105" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="105" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2521,64 +2531,161 @@
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+      <c r="A88" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B88">
-        <v>0.01</v>
-      </c>
-      <c r="C88">
-        <v>1000</v>
-      </c>
-      <c r="D88">
-        <v>5001</v>
-      </c>
-      <c r="E88">
-        <v>1530</v>
-      </c>
-      <c r="F88">
-        <v>1570</v>
-      </c>
-      <c r="G88">
+      <c r="B88" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="C88" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D88" s="4">
+        <v>5001</v>
+      </c>
+      <c r="E88" s="4">
+        <v>1530</v>
+      </c>
+      <c r="F88" s="4">
+        <v>1570</v>
+      </c>
+      <c r="G88" s="4">
         <v>1E-3</v>
       </c>
-      <c r="H88" t="s">
-        <v>30</v>
-      </c>
-      <c r="I88">
+      <c r="H88" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I88" s="4">
         <v>1</v>
       </c>
-      <c r="J88">
+      <c r="J88" s="4">
         <v>0.98282051282051597</v>
       </c>
-      <c r="K88">
+      <c r="K88" s="4">
         <v>5.5097596875867197E-3</v>
       </c>
-      <c r="L88" t="s">
+      <c r="L88" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="M88">
+      <c r="M88" s="4">
         <v>0.16184922620443801</v>
       </c>
-      <c r="N88">
+      <c r="N88" s="4">
         <v>6.0009599444959304E-3</v>
       </c>
-      <c r="O88">
+      <c r="O88" s="4">
         <v>9978.8525564459196</v>
       </c>
-      <c r="P88">
+      <c r="P88" s="4">
         <v>283.12224613964702</v>
       </c>
-      <c r="Q88">
+      <c r="Q88" s="4">
         <v>99366917.390740097</v>
       </c>
-      <c r="R88">
+      <c r="R88" s="4">
         <v>8460116.0168236997</v>
       </c>
-      <c r="S88">
+      <c r="S88" s="4">
         <v>100</v>
       </c>
-      <c r="T88">
+      <c r="T88" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="U88" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>51</v>
+      </c>
+      <c r="B89">
+        <v>0.01</v>
+      </c>
+      <c r="C89">
+        <v>1000</v>
+      </c>
+      <c r="D89">
+        <v>5001</v>
+      </c>
+      <c r="E89">
+        <v>1530</v>
+      </c>
+      <c r="F89">
+        <v>1570</v>
+      </c>
+      <c r="G89">
+        <v>1E-3</v>
+      </c>
+      <c r="H89" t="s">
+        <v>30</v>
+      </c>
+      <c r="I89">
+        <v>1</v>
+      </c>
+      <c r="U89" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>51</v>
+      </c>
+      <c r="B90">
+        <v>0.01</v>
+      </c>
+      <c r="C90">
+        <v>1000</v>
+      </c>
+      <c r="D90">
+        <v>5001</v>
+      </c>
+      <c r="E90">
+        <v>1530</v>
+      </c>
+      <c r="F90">
+        <v>1570</v>
+      </c>
+      <c r="G90">
+        <v>1.5E-3</v>
+      </c>
+      <c r="H90" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90">
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>0.98153846153846003</v>
+      </c>
+      <c r="K90">
+        <v>4.3858818636388196E-3</v>
+      </c>
+      <c r="L90" t="s">
+        <v>56</v>
+      </c>
+      <c r="M90">
+        <v>0.133427659342539</v>
+      </c>
+      <c r="N90">
+        <v>3.9535320072782501E-3</v>
+      </c>
+      <c r="O90">
+        <v>11915.510338869801</v>
+      </c>
+      <c r="P90">
+        <v>264.39216040517698</v>
+      </c>
+      <c r="Q90">
+        <v>169175684.93642601</v>
+      </c>
+      <c r="R90">
+        <v>11266552.773672201</v>
+      </c>
+      <c r="S90">
+        <v>100</v>
+      </c>
+      <c r="T90">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Q factor data run for sg_rr_100_028 2023-12-08 16-58-05.csv
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB8DA30-946D-4A3E-BB52-85A4F19A1F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7F391C-AA80-4B90-82D9-CFAB9129F5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="102">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -716,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:V90"/>
+  <dimension ref="A1:V91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="105" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="105" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2689,6 +2689,68 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>54</v>
+      </c>
+      <c r="B91">
+        <v>0.01</v>
+      </c>
+      <c r="C91">
+        <v>1000</v>
+      </c>
+      <c r="D91">
+        <v>5001</v>
+      </c>
+      <c r="E91">
+        <v>1530</v>
+      </c>
+      <c r="F91">
+        <v>1570</v>
+      </c>
+      <c r="G91">
+        <v>1E-3</v>
+      </c>
+      <c r="H91" t="s">
+        <v>30</v>
+      </c>
+      <c r="I91">
+        <v>1</v>
+      </c>
+      <c r="J91">
+        <v>0.98274999999999801</v>
+      </c>
+      <c r="K91">
+        <v>3.2814064370514399E-3</v>
+      </c>
+      <c r="L91" t="s">
+        <v>56</v>
+      </c>
+      <c r="M91">
+        <v>0.113844943291474</v>
+      </c>
+      <c r="N91">
+        <v>2.7215587843142401E-3</v>
+      </c>
+      <c r="O91">
+        <v>13870.8726906423</v>
+      </c>
+      <c r="P91">
+        <v>273.55330945369201</v>
+      </c>
+      <c r="Q91">
+        <v>266877129.125166</v>
+      </c>
+      <c r="R91">
+        <v>15798607.039031999</v>
+      </c>
+      <c r="S91">
+        <v>100</v>
+      </c>
+      <c r="T91">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Q factor run for sg_rr_100_030 2023-12-08 16-08-32.csv
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7F391C-AA80-4B90-82D9-CFAB9129F5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F3E6FC-7963-4B12-9D8C-98759AD795D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="102">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -716,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:V91"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="105" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="105" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2751,6 +2751,68 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>57</v>
+      </c>
+      <c r="B92">
+        <v>0.01</v>
+      </c>
+      <c r="C92">
+        <v>1000</v>
+      </c>
+      <c r="D92">
+        <v>5001</v>
+      </c>
+      <c r="E92">
+        <v>1530</v>
+      </c>
+      <c r="F92">
+        <v>1570</v>
+      </c>
+      <c r="G92">
+        <v>1E-3</v>
+      </c>
+      <c r="H92" t="s">
+        <v>30</v>
+      </c>
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <v>0.98128205128205004</v>
+      </c>
+      <c r="K92">
+        <v>3.16397329552258E-3</v>
+      </c>
+      <c r="L92" t="s">
+        <v>56</v>
+      </c>
+      <c r="M92">
+        <v>8.8124847759236999E-2</v>
+      </c>
+      <c r="N92">
+        <v>2.0009495564127801E-3</v>
+      </c>
+      <c r="O92">
+        <v>18076.149084442499</v>
+      </c>
+      <c r="P92">
+        <v>588.41920887440301</v>
+      </c>
+      <c r="Q92">
+        <v>590633048.05278397</v>
+      </c>
+      <c r="R92">
+        <v>57691387.464172103</v>
+      </c>
+      <c r="S92">
+        <v>100</v>
+      </c>
+      <c r="T92">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
repeat Q factor data run for sg_rr_100_025 2023-12-11 14-23-14
</commit_message>
<xml_diff>
--- a/data_analysis/fsr_data_analysis_table.xlsx
+++ b/data_analysis/fsr_data_analysis_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamCoding\Documents\Team_project\shared_git_repo\team-chip-project\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F3E6FC-7963-4B12-9D8C-98759AD795D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6BDF2D-13CF-42D7-B7F0-BFBB27B85DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B091661-B96C-465A-AF61-A63A653772E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="103">
   <si>
     <t>Data CSV filename</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>actually have reason to think I recorded approx fsr wrong on this one, so need to redo. Because when putting in for next run saw it to still be 1.7.</t>
+  </si>
+  <si>
+    <t>yes although possibly missed peak at end, but hard to tell if that's really a peak anyway.</t>
   </si>
 </sst>
 </file>
@@ -716,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C06AB-68A4-44B1-A92F-3D4C83DFB631}">
-  <dimension ref="A1:V92"/>
+  <dimension ref="A1:V94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="105" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="105" workbookViewId="0">
+      <selection activeCell="R94" sqref="R94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2813,6 +2816,100 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>48</v>
+      </c>
+      <c r="B93">
+        <v>0.01</v>
+      </c>
+      <c r="C93">
+        <v>1000</v>
+      </c>
+      <c r="D93">
+        <v>5001</v>
+      </c>
+      <c r="E93">
+        <v>1530</v>
+      </c>
+      <c r="F93">
+        <v>1570</v>
+      </c>
+      <c r="G93">
+        <v>1E-3</v>
+      </c>
+      <c r="H93" t="s">
+        <v>30</v>
+      </c>
+      <c r="I93">
+        <v>1</v>
+      </c>
+      <c r="U93" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>48</v>
+      </c>
+      <c r="B94">
+        <v>0.01</v>
+      </c>
+      <c r="C94">
+        <v>1000</v>
+      </c>
+      <c r="D94">
+        <v>5001</v>
+      </c>
+      <c r="E94">
+        <v>1530</v>
+      </c>
+      <c r="F94">
+        <v>1570</v>
+      </c>
+      <c r="G94">
+        <v>1.5E-3</v>
+      </c>
+      <c r="H94" t="s">
+        <v>30</v>
+      </c>
+      <c r="I94">
+        <v>1</v>
+      </c>
+      <c r="J94">
+        <v>0.98282051282051597</v>
+      </c>
+      <c r="K94">
+        <v>5.5097596875867197E-3</v>
+      </c>
+      <c r="L94" t="s">
+        <v>102</v>
+      </c>
+      <c r="M94">
+        <v>0.15507613665588901</v>
+      </c>
+      <c r="N94">
+        <v>4.7121321070659299E-3</v>
+      </c>
+      <c r="O94">
+        <v>10269.381068504999</v>
+      </c>
+      <c r="P94">
+        <v>236.72287624766</v>
+      </c>
+      <c r="Q94">
+        <v>108301085.330331</v>
+      </c>
+      <c r="R94">
+        <v>7492583.1937577203</v>
+      </c>
+      <c r="S94">
+        <v>100</v>
+      </c>
+      <c r="T94">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>